<commit_message>
html fieldset legend img input type name value
</commit_message>
<xml_diff>
--- a/introductionToJs/Practice Sheet_1_dev.xlsx
+++ b/introductionToJs/Practice Sheet_1_dev.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/da3dc409697ed301/Desktop/Pep Web dev/introductionToJs/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_3A7D436868EF837E3E37A6E514260243F1C63AA2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5E699913-9045-416A-B1E0-2787DA944F09}"/>
+  <bookViews>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="30">
   <si>
     <t>Practical Javscript Practice Sheet</t>
   </si>
@@ -26,9 +35,6 @@
   </si>
   <si>
     <t>Solve these on your vs code</t>
-  </si>
-  <si>
-    <t>Done</t>
   </si>
   <si>
     <t>https://www.pepcoding.com/resources/online-java-foundation/getting-started/print-all-primes-till-n-official/ojquestion</t>
@@ -109,93 +115,104 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="8">
-    <font>
-      <sz val="10.0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="36.0"/>
+      <sz val="36"/>
       <color theme="1"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="14.0"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF1155CC"/>
-    </font>
-    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
-    </font>
-    <font>
-      <sz val="14.0"/>
-    </font>
-    <font/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -385,24 +402,29 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="112.29"/>
-    <col customWidth="1" min="2" max="2" width="27.43"/>
+    <col min="1" max="1" width="112.26953125" customWidth="1"/>
+    <col min="2" max="2" width="27.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.85">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -410,242 +432,226 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="s">
+      <c r="B4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="5" t="s">
+      <c r="B5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="5" t="s">
+      <c r="B6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="4"/>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="5" t="s">
+      <c r="B7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="3" t="s">
+      <c r="B8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="3" t="s">
+      <c r="B9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="3" t="s">
+      <c r="B10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="4"/>
+    </row>
+    <row r="12" spans="1:3" ht="17.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="2" t="s">
+    </row>
+    <row r="13" spans="1:3" ht="17.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="2" t="s">
+    <row r="14" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="3" t="s">
+      <c r="B14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="4"/>
+    </row>
+    <row r="15" spans="1:3" ht="17.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="2" t="s">
+    </row>
+    <row r="16" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="5" t="s">
-        <v>17</v>
-      </c>
       <c r="B16" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="4"/>
+    </row>
+    <row r="17" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="5" t="s">
+      <c r="B17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="4"/>
+    </row>
+    <row r="18" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="3" t="s">
+      <c r="B18" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="4"/>
+    </row>
+    <row r="19" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="5" t="s">
+      <c r="B19" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="4"/>
+    </row>
+    <row r="20" spans="1:3" ht="17.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="6" t="s">
+    </row>
+    <row r="21" spans="1:3" ht="17.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="2" t="s">
+    <row r="22" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" s="5" t="s">
+    <row r="23" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="5" t="s">
+      <c r="B23" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="5" t="s">
+    </row>
+    <row r="25" spans="1:3" ht="17.5" x14ac:dyDescent="0.35">
+      <c r="A25" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" s="2" t="s">
+    <row r="26" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" s="5" t="s">
+    <row r="27" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" s="5" t="s">
+    <row r="28" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33">
+    <row r="33" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="A3"/>
-    <hyperlink r:id="rId2" ref="A4"/>
-    <hyperlink r:id="rId3" ref="A5"/>
-    <hyperlink r:id="rId4" ref="A6"/>
-    <hyperlink r:id="rId5" ref="A7"/>
-    <hyperlink r:id="rId6" ref="A8"/>
-    <hyperlink r:id="rId7" ref="A9"/>
-    <hyperlink r:id="rId8" ref="A10"/>
-    <hyperlink r:id="rId9" ref="A14"/>
-    <hyperlink r:id="rId10" ref="A16"/>
-    <hyperlink r:id="rId11" ref="A17"/>
-    <hyperlink r:id="rId12" ref="A18"/>
-    <hyperlink r:id="rId13" ref="A19"/>
-    <hyperlink r:id="rId14" ref="A22"/>
-    <hyperlink r:id="rId15" ref="A23"/>
-    <hyperlink r:id="rId16" ref="A24"/>
-    <hyperlink r:id="rId17" ref="A26"/>
-    <hyperlink r:id="rId18" ref="A27"/>
-    <hyperlink r:id="rId19" ref="A28"/>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="A6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="A7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="A8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="A9" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="A10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="A14" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="A16" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="A17" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="A18" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="A19" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="A22" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="A23" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="A24" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="A26" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="A27" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="A28" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
   </hyperlinks>
-  <drawing r:id="rId20"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>